<commit_message>
Updated Sensor Calibration Updated Sensor Calibration to match the other thermometers I'm using for this project.
</commit_message>
<xml_diff>
--- a/SensorCalibration.xlsx
+++ b/SensorCalibration.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Pi Temp</t>
   </si>
@@ -55,18 +55,45 @@
   <si>
     <t>Real</t>
   </si>
+  <si>
+    <t>Dec 19, 2023 observations (freezer and fridge test)</t>
+  </si>
+  <si>
+    <t>PiTemp</t>
+  </si>
+  <si>
+    <t>Pi Sensor</t>
+  </si>
+  <si>
+    <t>Calculated</t>
+  </si>
+  <si>
+    <t>Remote Themomoeter</t>
+  </si>
+  <si>
+    <t>Red Themomoeter</t>
+  </si>
+  <si>
+    <t>Grey Themomoeter</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -77,7 +104,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -85,12 +112,143 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -237,11 +395,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="44090112"/>
-        <c:axId val="44091648"/>
+        <c:axId val="254023168"/>
+        <c:axId val="254024704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="44090112"/>
+        <c:axId val="254023168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -250,7 +408,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44091648"/>
+        <c:crossAx val="254024704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -258,7 +416,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44091648"/>
+        <c:axId val="254024704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -269,7 +427,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44090112"/>
+        <c:crossAx val="254023168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -467,11 +625,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="141965568"/>
-        <c:axId val="141967360"/>
+        <c:axId val="254045568"/>
+        <c:axId val="254059648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="141965568"/>
+        <c:axId val="254045568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -480,7 +638,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141967360"/>
+        <c:crossAx val="254059648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -488,7 +646,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141967360"/>
+        <c:axId val="254059648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -499,7 +657,295 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141965568"/>
+        <c:crossAx val="254045568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$68</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PiTemp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$69:$A$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$68</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pi Sensor</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$69:$B$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$68</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Calculated</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$69:$C$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>15.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42.08</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$68</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remote Themomoeter</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$69:$D$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$68</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Red Themomoeter</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$69:$E$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$68</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Grey Themomoeter</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$69:$F$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="52885760"/>
+        <c:axId val="52953088"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="52885760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="52953088"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="52953088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="52885760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -578,6 +1024,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>328612</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>23812</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -873,10 +1349,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D62"/>
+  <dimension ref="A2:P82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="U70" sqref="U70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,13 +1450,13 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <f>(((B17-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" ref="C17:C62" si="0">(((B17-RawLow)*RefRange)/RawRange)+RefLow</f>
         <v>38.752855659397717</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" ref="A18:A62" si="0">(B18*9/5)+32</f>
+        <f t="shared" ref="A18:A62" si="1">(B18*9/5)+32</f>
         <v>33.799999999999997</v>
       </c>
       <c r="B18">
@@ -988,632 +1464,972 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <f>(((B18-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>39.895119418483901</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35.6</v>
       </c>
       <c r="B19">
-        <f t="shared" ref="B19:B62" si="1">B18+1</f>
+        <f t="shared" ref="B19:B62" si="2">B18+1</f>
         <v>2</v>
       </c>
       <c r="C19">
-        <f>(((B19-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>41.037383177570092</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37.4</v>
       </c>
       <c r="B20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C20">
-        <f>(((B20-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>42.179646936656283</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39.200000000000003</v>
       </c>
       <c r="B21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="C21">
-        <f>(((B21-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>43.321910695742474</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="B22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="C22">
-        <f>(((B22-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>44.464174454828658</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42.8</v>
       </c>
       <c r="B23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="C23">
-        <f>(((B23-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>45.606438213914849</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44.6</v>
       </c>
       <c r="B24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="C24">
-        <f>(((B24-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>46.74870197300104</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46.4</v>
       </c>
       <c r="B25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="C25">
-        <f>(((B25-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>47.890965732087224</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48.2</v>
       </c>
       <c r="B26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="C26">
-        <f>(((B26-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>49.033229491173415</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="B27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="C27">
-        <f>(((B27-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>50.175493250259606</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>51.8</v>
       </c>
       <c r="B28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="C28">
-        <f>(((B28-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>51.317757009345797</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>53.6</v>
       </c>
       <c r="B29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="C29">
-        <f>(((B29-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>52.460020768431981</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>55.4</v>
       </c>
       <c r="B30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="C30">
-        <f>(((B30-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>53.602284527518172</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>57.2</v>
       </c>
       <c r="B31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="C31">
-        <f>(((B31-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>54.744548286604363</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>59</v>
       </c>
       <c r="B32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="C32">
-        <f>(((B32-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>55.886812045690547</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>60.8</v>
       </c>
       <c r="B33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="C33">
-        <f>(((B33-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>57.029075804776738</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>62.6</v>
       </c>
       <c r="B34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="C34">
-        <f>(((B34-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>58.171339563862929</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>64.400000000000006</v>
       </c>
       <c r="B35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="C35">
-        <f>(((B35-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>59.31360332294912</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>66.2</v>
       </c>
       <c r="B36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="C36">
-        <f>(((B36-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>60.455867082035304</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>68</v>
       </c>
       <c r="B37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="C37">
-        <f>(((B37-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>61.598130841121495</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>69.8</v>
       </c>
       <c r="B38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="C38">
-        <f>(((B38-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>62.740394600207686</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>71.599999999999994</v>
       </c>
       <c r="B39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="C39">
-        <f>(((B39-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>63.88265835929387</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>73.400000000000006</v>
       </c>
       <c r="B40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="C40">
-        <f>(((B40-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>65.024922118380061</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>75.2</v>
       </c>
       <c r="B41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="C41">
-        <f>(((B41-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>66.167185877466252</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>77</v>
       </c>
       <c r="B42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="C42">
-        <f>(((B42-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>67.309449636552444</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>78.8</v>
       </c>
       <c r="B43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="C43">
-        <f>(((B43-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>68.45171339563862</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>80.599999999999994</v>
       </c>
       <c r="B44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="C44">
-        <f>(((B44-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>69.593977154724826</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>82.4</v>
       </c>
       <c r="B45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="C45">
-        <f>(((B45-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>70.736240913811002</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>84.2</v>
       </c>
       <c r="B46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
       <c r="C46">
-        <f>(((B46-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>71.878504672897193</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>86</v>
       </c>
       <c r="B47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="C47">
-        <f>(((B47-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>73.020768431983385</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>87.8</v>
       </c>
       <c r="B48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="C48">
-        <f>(((B48-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>74.163032191069576</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>89.6</v>
       </c>
       <c r="B49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="C49">
-        <f>(((B49-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>75.305295950155767</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>91.4</v>
       </c>
       <c r="B50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
       <c r="C50">
-        <f>(((B50-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>76.447559709241943</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>93.2</v>
       </c>
       <c r="B51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="C51">
-        <f>(((B51-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>77.589823468328149</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>95</v>
       </c>
       <c r="B52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="C52">
-        <f>(((B52-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>78.732087227414326</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>96.8</v>
       </c>
       <c r="B53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="C53">
-        <f>(((B53-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>79.874350986500517</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>98.6</v>
       </c>
       <c r="B54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
       <c r="C54">
-        <f>(((B54-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>81.016614745586708</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100.4</v>
       </c>
       <c r="B55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="C55">
-        <f>(((B55-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>82.158878504672899</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>102.2</v>
       </c>
       <c r="B56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="C56">
-        <f>(((B56-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>83.30114226375909</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
       <c r="B57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="C57">
-        <f>(((B57-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>84.443406022845267</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>105.8</v>
       </c>
       <c r="B58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
       <c r="C58">
-        <f>(((B58-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>85.585669781931472</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>107.6</v>
       </c>
       <c r="B59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>42</v>
       </c>
       <c r="C59">
-        <f>(((B59-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>86.727933541017649</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>109.4</v>
       </c>
       <c r="B60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="C60">
-        <f>(((B60-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>87.87019730010384</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>111.2</v>
       </c>
       <c r="B61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="C61">
-        <f>(((B61-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>89.012461059190031</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>113</v>
       </c>
       <c r="B62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="C62">
-        <f>(((B62-RawLow)*RefRange)/RawRange)+RefLow</f>
+        <f t="shared" si="0"/>
         <v>90.154724818276222</v>
       </c>
+    </row>
+    <row r="65" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
+      <c r="J66" s="4"/>
+      <c r="K66" s="4"/>
+      <c r="L66" s="4"/>
+      <c r="M66" s="4"/>
+      <c r="N66" s="4"/>
+      <c r="O66" s="4"/>
+      <c r="P66" s="5"/>
+    </row>
+    <row r="67" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="6"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
+      <c r="G67" s="7"/>
+      <c r="H67" s="7"/>
+      <c r="I67" s="7"/>
+      <c r="J67" s="7"/>
+      <c r="K67" s="7"/>
+      <c r="L67" s="7"/>
+      <c r="M67" s="7"/>
+      <c r="N67" s="7"/>
+      <c r="O67" s="7"/>
+      <c r="P67" s="8"/>
+    </row>
+    <row r="68" spans="1:16" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G68" s="7"/>
+      <c r="H68" s="7"/>
+      <c r="I68" s="7"/>
+      <c r="J68" s="7"/>
+      <c r="K68" s="7"/>
+      <c r="L68" s="7"/>
+      <c r="M68" s="7"/>
+      <c r="N68" s="7"/>
+      <c r="O68" s="7"/>
+      <c r="P68" s="8"/>
+    </row>
+    <row r="69" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="10">
+        <v>28</v>
+      </c>
+      <c r="B69" s="2">
+        <v>-9</v>
+      </c>
+      <c r="C69" s="2">
+        <v>15.8</v>
+      </c>
+      <c r="D69" s="2">
+        <v>-3</v>
+      </c>
+      <c r="E69" s="2">
+        <v>-12</v>
+      </c>
+      <c r="F69" s="2">
+        <v>-4</v>
+      </c>
+      <c r="G69" s="7"/>
+      <c r="H69" s="7"/>
+      <c r="I69" s="7"/>
+      <c r="J69" s="7"/>
+      <c r="K69" s="7"/>
+      <c r="L69" s="7"/>
+      <c r="M69" s="7"/>
+      <c r="N69" s="7"/>
+      <c r="O69" s="7"/>
+      <c r="P69" s="8"/>
+    </row>
+    <row r="70" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="10">
+        <v>45</v>
+      </c>
+      <c r="B70" s="2">
+        <v>5.6</v>
+      </c>
+      <c r="C70" s="2">
+        <v>42.08</v>
+      </c>
+      <c r="D70" s="2">
+        <v>20</v>
+      </c>
+      <c r="E70" s="2">
+        <v>28</v>
+      </c>
+      <c r="F70" s="2">
+        <v>22</v>
+      </c>
+      <c r="G70" s="7"/>
+      <c r="H70" s="7"/>
+      <c r="I70" s="7"/>
+      <c r="J70" s="7"/>
+      <c r="K70" s="7"/>
+      <c r="L70" s="7"/>
+      <c r="M70" s="7"/>
+      <c r="N70" s="7"/>
+      <c r="O70" s="7"/>
+      <c r="P70" s="8"/>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A71" s="6"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
+      <c r="I71" s="7"/>
+      <c r="J71" s="7"/>
+      <c r="K71" s="7"/>
+      <c r="L71" s="7"/>
+      <c r="M71" s="7"/>
+      <c r="N71" s="7"/>
+      <c r="O71" s="7"/>
+      <c r="P71" s="8"/>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A72" s="6"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="7"/>
+      <c r="F72" s="7"/>
+      <c r="G72" s="7"/>
+      <c r="H72" s="7"/>
+      <c r="I72" s="7"/>
+      <c r="J72" s="7"/>
+      <c r="K72" s="7"/>
+      <c r="L72" s="7"/>
+      <c r="M72" s="7"/>
+      <c r="N72" s="7"/>
+      <c r="O72" s="7"/>
+      <c r="P72" s="8"/>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A73" s="6"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
+      <c r="F73" s="7"/>
+      <c r="G73" s="7"/>
+      <c r="H73" s="7"/>
+      <c r="I73" s="7"/>
+      <c r="J73" s="7"/>
+      <c r="K73" s="7"/>
+      <c r="L73" s="7"/>
+      <c r="M73" s="7"/>
+      <c r="N73" s="7"/>
+      <c r="O73" s="7"/>
+      <c r="P73" s="8"/>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A74" s="6"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
+      <c r="H74" s="7"/>
+      <c r="I74" s="7"/>
+      <c r="J74" s="7"/>
+      <c r="K74" s="7"/>
+      <c r="L74" s="7"/>
+      <c r="M74" s="7"/>
+      <c r="N74" s="7"/>
+      <c r="O74" s="7"/>
+      <c r="P74" s="8"/>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A75" s="6"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7"/>
+      <c r="H75" s="7"/>
+      <c r="I75" s="7"/>
+      <c r="J75" s="7"/>
+      <c r="K75" s="7"/>
+      <c r="L75" s="7"/>
+      <c r="M75" s="7"/>
+      <c r="N75" s="7"/>
+      <c r="O75" s="7"/>
+      <c r="P75" s="8"/>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A76" s="6"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="7"/>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
+      <c r="H76" s="7"/>
+      <c r="I76" s="7"/>
+      <c r="J76" s="7"/>
+      <c r="K76" s="7"/>
+      <c r="L76" s="7"/>
+      <c r="M76" s="7"/>
+      <c r="N76" s="7"/>
+      <c r="O76" s="7"/>
+      <c r="P76" s="8"/>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A77" s="6"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="7"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="7"/>
+      <c r="H77" s="7"/>
+      <c r="I77" s="7"/>
+      <c r="J77" s="7"/>
+      <c r="K77" s="7"/>
+      <c r="L77" s="7"/>
+      <c r="M77" s="7"/>
+      <c r="N77" s="7"/>
+      <c r="O77" s="7"/>
+      <c r="P77" s="8"/>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A78" s="6"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="7"/>
+      <c r="I78" s="7"/>
+      <c r="J78" s="7"/>
+      <c r="K78" s="7"/>
+      <c r="L78" s="7"/>
+      <c r="M78" s="7"/>
+      <c r="N78" s="7"/>
+      <c r="O78" s="7"/>
+      <c r="P78" s="8"/>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G79" s="7"/>
+      <c r="H79" s="7"/>
+      <c r="I79" s="7"/>
+      <c r="J79" s="7"/>
+      <c r="K79" s="7"/>
+      <c r="L79" s="7"/>
+      <c r="M79" s="7"/>
+      <c r="N79" s="7"/>
+      <c r="O79" s="7"/>
+      <c r="P79" s="8"/>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A80" s="6"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7"/>
+      <c r="H80" s="7"/>
+      <c r="I80" s="7"/>
+      <c r="J80" s="7"/>
+      <c r="K80" s="7"/>
+      <c r="L80" s="7"/>
+      <c r="M80" s="7"/>
+      <c r="N80" s="7"/>
+      <c r="O80" s="7"/>
+      <c r="P80" s="8"/>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A81" s="6"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="7"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
+      <c r="H81" s="7"/>
+      <c r="I81" s="7"/>
+      <c r="J81" s="7"/>
+      <c r="K81" s="7"/>
+      <c r="L81" s="7"/>
+      <c r="M81" s="7"/>
+      <c r="N81" s="7"/>
+      <c r="O81" s="7"/>
+      <c r="P81" s="8"/>
+    </row>
+    <row r="82" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="11"/>
+      <c r="B82" s="12"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="12"/>
+      <c r="E82" s="12"/>
+      <c r="F82" s="12"/>
+      <c r="G82" s="12"/>
+      <c r="H82" s="12"/>
+      <c r="I82" s="12"/>
+      <c r="J82" s="12"/>
+      <c r="K82" s="12"/>
+      <c r="L82" s="12"/>
+      <c r="M82" s="12"/>
+      <c r="N82" s="12"/>
+      <c r="O82" s="12"/>
+      <c r="P82" s="13"/>
     </row>
   </sheetData>
   <sortState ref="B3:C5">
     <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Save Data as CSV and Graph it Save data as a CSV file, then graph it, and push the graph to Amazon S3 bucket for web access
</commit_message>
<xml_diff>
--- a/SensorCalibration.xlsx
+++ b/SensorCalibration.xlsx
@@ -12,19 +12,19 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="RawHigh">Sheet1!$B$13</definedName>
-    <definedName name="RawLow">Sheet1!$B$12</definedName>
-    <definedName name="RawRange">Sheet1!$B$14</definedName>
-    <definedName name="RefHi">Sheet1!$C$13</definedName>
-    <definedName name="RefLow">Sheet1!$C$12</definedName>
-    <definedName name="RefRange">Sheet1!$C$14</definedName>
+    <definedName name="RawHigh">Sheet1!$D$13</definedName>
+    <definedName name="RawLow">Sheet1!$D$12</definedName>
+    <definedName name="RawRange">Sheet1!$D$14</definedName>
+    <definedName name="RefHi">Sheet1!$E$13</definedName>
+    <definedName name="RefLow">Sheet1!$E$12</definedName>
+    <definedName name="RefRange">Sheet1!$E$14</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
   <si>
     <t>Pi Temp</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Pi Sensor</t>
   </si>
   <si>
-    <t>Calculated</t>
-  </si>
-  <si>
     <t>Remote Themomoeter</t>
   </si>
   <si>
@@ -75,13 +72,175 @@
   </si>
   <si>
     <t>Grey Themomoeter</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>9:00pm</t>
+  </si>
+  <si>
+    <t>3:00pm</t>
+  </si>
+  <si>
+    <t>C to F Conversion</t>
+  </si>
+  <si>
+    <t>New Formula</t>
+  </si>
+  <si>
+    <t>9:50m</t>
+  </si>
+  <si>
+    <t>10:30pm</t>
+  </si>
+  <si>
+    <t>8:12am</t>
+  </si>
+  <si>
+    <t>8:20am</t>
+  </si>
+  <si>
+    <t>8:30am</t>
+  </si>
+  <si>
+    <t>8:34am</t>
+  </si>
+  <si>
+    <t>8:42am</t>
+  </si>
+  <si>
+    <t>8:45am</t>
+  </si>
+  <si>
+    <t>8:52am</t>
+  </si>
+  <si>
+    <t>8:48am</t>
+  </si>
+  <si>
+    <t>9:03am</t>
+  </si>
+  <si>
+    <t>8:55am</t>
+  </si>
+  <si>
+    <t>8:58am</t>
+  </si>
+  <si>
+    <t>9:08am</t>
+  </si>
+  <si>
+    <t>9:19am</t>
+  </si>
+  <si>
+    <t>9:14am</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>9:31am</t>
+  </si>
+  <si>
+    <t>9:25am</t>
+  </si>
+  <si>
+    <t>9:36am</t>
+  </si>
+  <si>
+    <t>9:40am</t>
+  </si>
+  <si>
+    <t>10:08am</t>
+  </si>
+  <si>
+    <t>9:45am</t>
+  </si>
+  <si>
+    <t>10:10am</t>
+  </si>
+  <si>
+    <t>10:25am</t>
+  </si>
+  <si>
+    <t>10:37am</t>
+  </si>
+  <si>
+    <t>12:06am</t>
+  </si>
+  <si>
+    <t>1:54pm</t>
+  </si>
+  <si>
+    <t>7:55am</t>
+  </si>
+  <si>
+    <t>8:02am</t>
+  </si>
+  <si>
+    <t>8:14am</t>
+  </si>
+  <si>
+    <t>"=(D70*1.9)+16.5</t>
+  </si>
+  <si>
+    <t>Factor</t>
+  </si>
+  <si>
+    <t>Adjustment</t>
+  </si>
+  <si>
+    <t>8:21am</t>
+  </si>
+  <si>
+    <t>8:54am</t>
+  </si>
+  <si>
+    <t>8:57am</t>
+  </si>
+  <si>
+    <t>11:28am</t>
+  </si>
+  <si>
+    <t>10:35am</t>
+  </si>
+  <si>
+    <t>12:34am</t>
+  </si>
+  <si>
+    <t>1:40pm</t>
+  </si>
+  <si>
+    <t>2:06pm</t>
+  </si>
+  <si>
+    <t>2:50pm</t>
+  </si>
+  <si>
+    <t>1:45pm</t>
+  </si>
+  <si>
+    <t>12/24/223</t>
+  </si>
+  <si>
+    <t>3:05pm</t>
+  </si>
+  <si>
+    <t>Alarm  If the sensor reads 9.33 or lower - that is dangerously close to freezing in real life.</t>
+  </si>
+  <si>
+    <t>If the remote themometer hits 40 it's actually 30 in the real world!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,36 +254,56 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="7">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -177,80 +356,67 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -288,7 +454,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$2</c:f>
+              <c:f>Sheet1!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -302,7 +468,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$4</c:f>
+              <c:f>Sheet1!$D$3:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -322,7 +488,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$2</c:f>
+              <c:f>Sheet1!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -336,7 +502,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$4</c:f>
+              <c:f>Sheet1!$E$3:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -356,7 +522,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$2</c:f>
+              <c:f>Sheet1!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -370,7 +536,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$4</c:f>
+              <c:f>Sheet1!$F$3:$F$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -395,11 +561,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="254023168"/>
-        <c:axId val="254024704"/>
+        <c:axId val="180173824"/>
+        <c:axId val="180180864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="254023168"/>
+        <c:axId val="180173824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -408,7 +574,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="254024704"/>
+        <c:crossAx val="180180864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -416,7 +582,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="254024704"/>
+        <c:axId val="180180864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -427,7 +593,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="254023168"/>
+        <c:crossAx val="180173824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -474,7 +640,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$16</c:f>
+              <c:f>Sheet1!$D$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -488,7 +654,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$17:$B$31</c:f>
+              <c:f>Sheet1!$D$17:$D$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -547,7 +713,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$16</c:f>
+              <c:f>Sheet1!$E$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -561,7 +727,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$31</c:f>
+              <c:f>Sheet1!$E$17:$E$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -625,11 +791,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="254045568"/>
-        <c:axId val="254059648"/>
+        <c:axId val="302119168"/>
+        <c:axId val="302002176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="254045568"/>
+        <c:axId val="302119168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -638,7 +804,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="254059648"/>
+        <c:crossAx val="302002176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -646,7 +812,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="254059648"/>
+        <c:axId val="302002176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -657,7 +823,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="254045568"/>
+        <c:crossAx val="302119168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -704,7 +870,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$68</c:f>
+              <c:f>Sheet1!$C$68</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -718,10 +884,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$69:$A$70</c:f>
+              <c:f>Sheet1!$C$69:$C$112</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>28</c:v>
                 </c:pt>
@@ -738,7 +904,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$68</c:f>
+              <c:f>Sheet1!$D$68</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -752,15 +918,141 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$69:$B$70</c:f>
+              <c:f>Sheet1!$D$69:$D$112</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>-9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25.31</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.8478999999999992</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.08</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.6370000000000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.8734</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.1111</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.757100000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17.616599999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19.024799999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19.481999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20.1587</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20.7439</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20.160299999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21.7681</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22.389900000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>22.956800000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>23.340900000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>23.889500000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>24.346699999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>24.803899999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>25.242799999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>25.809799999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>26.285299999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26.8705</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>28.333600000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28.553000000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29.211400000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29.430900000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>32.667900000000003</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>28.882200000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8.3627000000000002</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>9.5513999999999992</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9.4050999999999991</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8.4541000000000004</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9.6611999999999991</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9.5879999999999992</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>10.411</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>10.91</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>10.7768</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>10.9779</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>9.33</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.37659</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -772,11 +1064,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$68</c:f>
+              <c:f>Sheet1!$E$68</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Calculated</c:v>
+                  <c:v>C to F Conversion</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -786,15 +1078,141 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$69:$C$70</c:f>
+              <c:f>Sheet1!$E$69:$E$112</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>15.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>42.08</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>77.557999999999993</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49.726219999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.143999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>47.546599999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>58.772120000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>59.199979999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>62.162780000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>63.709879999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>66.244640000000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>67.067599999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>68.285660000000007</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>69.339020000000005</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>68.288539999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>71.182580000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>72.301820000000006</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>73.322239999999994</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>74.013620000000003</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>75.001100000000008</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>75.824060000000003</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>76.647019999999998</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>77.437039999999996</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>78.457639999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>79.313540000000003</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>80.366900000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>83.000479999999996</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>83.395400000000009</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>84.580520000000007</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>84.975620000000006</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>90.802220000000005</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>83.987960000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>47.052860000000003</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>49.192520000000002</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>48.929180000000002</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>47.217379999999999</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>49.390159999999995</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>49.258399999999995</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>50.739800000000002</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>51.637999999999998</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>51.398240000000001</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>51.760220000000004</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>48.793999999999997</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>34.477862000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -806,7 +1224,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$68</c:f>
+              <c:f>Sheet1!$F$68</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -820,15 +1238,141 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$69:$D$70</c:f>
+              <c:f>Sheet1!$F$69:$F$112</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>46.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>49.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>52.3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>53.22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>56.8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>58.1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>59.4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>60.3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>62.2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>64.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>65.3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>66.2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>67.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>70.7</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>72.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>77.7</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>76.3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>38.5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>39.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>39.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>38.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>40.1</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>39.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>41.2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>41.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41.7</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41.7</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>40.5</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>30.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -840,7 +1384,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$68</c:f>
+              <c:f>Sheet1!$G$68</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -854,15 +1398,24 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$69:$E$70</c:f>
+              <c:f>Sheet1!$G$69:$G$112</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>-12</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -874,7 +1427,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$68</c:f>
+              <c:f>Sheet1!$H$68</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -888,15 +1441,184 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$69:$F$70</c:f>
+              <c:f>Sheet1!$H$69:$H$112</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$68</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>New Formula</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$69:$I$112</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="44"/>
+                <c:pt idx="0">
+                  <c:v>-0.59999999999999787</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27.14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64.588999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35.211010000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35.652000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.910299999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44.759460000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45.211089999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48.33849</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>49.971539999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>52.647119999999994</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>53.515799999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>54.80153</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>55.913409999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>54.804569999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>57.859389999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>59.04081</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>60.117919999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>60.847709999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>61.890050000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>62.758729999999993</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>63.627409999999998</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>64.461320000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>65.538619999999995</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>66.442070000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>67.55395</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>70.333839999999995</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>70.750699999999995</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>72.001660000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>72.418710000000004</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>78.569010000000006</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>71.376180000000005</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32.389130000000002</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34.647660000000002</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34.369689999999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>32.56279</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>34.856279999999998</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>34.717199999999998</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>36.280900000000003</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>37.228999999999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>36.975920000000002</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>37.35801</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>34.227000000000004</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>19.115521000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -913,11 +1635,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="52885760"/>
-        <c:axId val="52953088"/>
+        <c:axId val="302014848"/>
+        <c:axId val="302016384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="52885760"/>
+        <c:axId val="302014848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -926,7 +1648,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52953088"/>
+        <c:crossAx val="302016384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -934,7 +1656,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52953088"/>
+        <c:axId val="302016384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -945,7 +1667,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52885760"/>
+        <c:crossAx val="302014848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -971,13 +1693,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>271462</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>576262</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -1001,13 +1723,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>166687</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>471487</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -1031,15 +1753,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>328612</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>233362</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>23812</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>538162</xdr:colOff>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1349,1083 +2071,2218 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P82"/>
+  <dimension ref="A2:U114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="U70" sqref="U70"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="K108" sqref="K108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3">
+    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D3">
         <v>45</v>
       </c>
-      <c r="C3">
+      <c r="E3">
         <v>47</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>1.0444443999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4">
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D4">
         <v>97</v>
       </c>
-      <c r="C4">
+      <c r="E4">
         <v>80</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>0.82474226799999995</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
         <v>3</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
         <v>4</v>
       </c>
-      <c r="B12">
+      <c r="D12">
         <v>7.22</v>
       </c>
-      <c r="C12">
+      <c r="E12">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
         <v>5</v>
       </c>
-      <c r="B13">
+      <c r="D13">
         <v>36.11</v>
       </c>
-      <c r="C13">
+      <c r="E13">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
         <v>7</v>
       </c>
-      <c r="B14">
-        <f>B13-B12</f>
+      <c r="D14">
+        <f>D13-D12</f>
         <v>28.89</v>
       </c>
-      <c r="C14">
-        <f>C13-C12</f>
+      <c r="E14">
+        <f>E13-E12</f>
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
         <v>8</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f>(B17*9/5)+32</f>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <f>(D17*9/5)+32</f>
         <v>32</v>
       </c>
-      <c r="B17">
+      <c r="D17">
         <v>0</v>
       </c>
-      <c r="C17">
-        <f t="shared" ref="C17:C62" si="0">(((B17-RawLow)*RefRange)/RawRange)+RefLow</f>
+      <c r="E17">
+        <f t="shared" ref="E17:E62" si="0">(((D17-RawLow)*RefRange)/RawRange)+RefLow</f>
         <v>38.752855659397717</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <f t="shared" ref="A18:A62" si="1">(B18*9/5)+32</f>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <f t="shared" ref="C18:C62" si="1">(D18*9/5)+32</f>
         <v>33.799999999999997</v>
       </c>
-      <c r="B18">
-        <f>B17+1</f>
+      <c r="D18">
+        <f>D17+1</f>
         <v>1</v>
       </c>
-      <c r="C18">
+      <c r="E18">
         <f t="shared" si="0"/>
         <v>39.895119418483901</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C19">
         <f t="shared" si="1"/>
         <v>35.6</v>
       </c>
-      <c r="B19">
-        <f t="shared" ref="B19:B62" si="2">B18+1</f>
+      <c r="D19">
+        <f t="shared" ref="D19:D62" si="2">D18+1</f>
         <v>2</v>
       </c>
-      <c r="C19">
+      <c r="E19">
         <f t="shared" si="0"/>
         <v>41.037383177570092</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C20">
         <f t="shared" si="1"/>
         <v>37.4</v>
       </c>
-      <c r="B20">
+      <c r="D20">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="C20">
+      <c r="E20">
         <f t="shared" si="0"/>
         <v>42.179646936656283</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C21">
         <f t="shared" si="1"/>
         <v>39.200000000000003</v>
       </c>
-      <c r="B21">
+      <c r="D21">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="C21">
+      <c r="E21">
         <f t="shared" si="0"/>
         <v>43.321910695742474</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C22">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="B22">
+      <c r="D22">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="C22">
+      <c r="E22">
         <f t="shared" si="0"/>
         <v>44.464174454828658</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C23">
         <f t="shared" si="1"/>
         <v>42.8</v>
       </c>
-      <c r="B23">
+      <c r="D23">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="C23">
+      <c r="E23">
         <f t="shared" si="0"/>
         <v>45.606438213914849</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C24">
         <f t="shared" si="1"/>
         <v>44.6</v>
       </c>
-      <c r="B24">
+      <c r="D24">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="C24">
+      <c r="E24">
         <f t="shared" si="0"/>
         <v>46.74870197300104</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C25">
         <f t="shared" si="1"/>
         <v>46.4</v>
       </c>
-      <c r="B25">
+      <c r="D25">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="C25">
+      <c r="E25">
         <f t="shared" si="0"/>
         <v>47.890965732087224</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C26">
         <f t="shared" si="1"/>
         <v>48.2</v>
       </c>
-      <c r="B26">
+      <c r="D26">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="C26">
+      <c r="E26">
         <f t="shared" si="0"/>
         <v>49.033229491173415</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C27">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="B27">
+      <c r="D27">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="C27">
+      <c r="E27">
         <f t="shared" si="0"/>
         <v>50.175493250259606</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C28">
         <f t="shared" si="1"/>
         <v>51.8</v>
       </c>
-      <c r="B28">
+      <c r="D28">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="C28">
+      <c r="E28">
         <f t="shared" si="0"/>
         <v>51.317757009345797</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C29">
         <f t="shared" si="1"/>
         <v>53.6</v>
       </c>
-      <c r="B29">
+      <c r="D29">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="C29">
+      <c r="E29">
         <f t="shared" si="0"/>
         <v>52.460020768431981</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C30">
         <f t="shared" si="1"/>
         <v>55.4</v>
       </c>
-      <c r="B30">
+      <c r="D30">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="C30">
+      <c r="E30">
         <f t="shared" si="0"/>
         <v>53.602284527518172</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C31">
         <f t="shared" si="1"/>
         <v>57.2</v>
       </c>
-      <c r="B31">
+      <c r="D31">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="C31">
+      <c r="E31">
         <f t="shared" si="0"/>
         <v>54.744548286604363</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C32">
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
-      <c r="B32">
+      <c r="D32">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="C32">
+      <c r="E32">
         <f t="shared" si="0"/>
         <v>55.886812045690547</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C33">
         <f t="shared" si="1"/>
         <v>60.8</v>
       </c>
-      <c r="B33">
+      <c r="D33">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="C33">
+      <c r="E33">
         <f t="shared" si="0"/>
         <v>57.029075804776738</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34">
         <f t="shared" si="1"/>
         <v>62.6</v>
       </c>
-      <c r="B34">
+      <c r="D34">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="C34">
+      <c r="E34">
         <f t="shared" si="0"/>
         <v>58.171339563862929</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C35">
         <f t="shared" si="1"/>
         <v>64.400000000000006</v>
       </c>
-      <c r="B35">
+      <c r="D35">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="C35">
+      <c r="E35">
         <f t="shared" si="0"/>
         <v>59.31360332294912</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C36">
         <f t="shared" si="1"/>
         <v>66.2</v>
       </c>
-      <c r="B36">
+      <c r="D36">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="C36">
+      <c r="E36">
         <f t="shared" si="0"/>
         <v>60.455867082035304</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C37">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-      <c r="B37">
+      <c r="D37">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="C37">
+      <c r="E37">
         <f t="shared" si="0"/>
         <v>61.598130841121495</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C38">
         <f t="shared" si="1"/>
         <v>69.8</v>
       </c>
-      <c r="B38">
+      <c r="D38">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="C38">
+      <c r="E38">
         <f t="shared" si="0"/>
         <v>62.740394600207686</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C39">
         <f t="shared" si="1"/>
         <v>71.599999999999994</v>
       </c>
-      <c r="B39">
+      <c r="D39">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="C39">
+      <c r="E39">
         <f t="shared" si="0"/>
         <v>63.88265835929387</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40">
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C40">
         <f t="shared" si="1"/>
         <v>73.400000000000006</v>
       </c>
-      <c r="B40">
+      <c r="D40">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="C40">
+      <c r="E40">
         <f t="shared" si="0"/>
         <v>65.024922118380061</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41">
+    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C41">
         <f t="shared" si="1"/>
         <v>75.2</v>
       </c>
-      <c r="B41">
+      <c r="D41">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="C41">
+      <c r="E41">
         <f t="shared" si="0"/>
         <v>66.167185877466252</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42">
+    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C42">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
-      <c r="B42">
+      <c r="D42">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="C42">
+      <c r="E42">
         <f t="shared" si="0"/>
         <v>67.309449636552444</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43">
+    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C43">
         <f t="shared" si="1"/>
         <v>78.8</v>
       </c>
-      <c r="B43">
+      <c r="D43">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="C43">
+      <c r="E43">
         <f t="shared" si="0"/>
         <v>68.45171339563862</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44">
+    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C44">
         <f t="shared" si="1"/>
         <v>80.599999999999994</v>
       </c>
-      <c r="B44">
+      <c r="D44">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="C44">
+      <c r="E44">
         <f t="shared" si="0"/>
         <v>69.593977154724826</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45">
+    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C45">
         <f t="shared" si="1"/>
         <v>82.4</v>
       </c>
-      <c r="B45">
+      <c r="D45">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="C45">
+      <c r="E45">
         <f t="shared" si="0"/>
         <v>70.736240913811002</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46">
+    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C46">
         <f t="shared" si="1"/>
         <v>84.2</v>
       </c>
-      <c r="B46">
+      <c r="D46">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="C46">
+      <c r="E46">
         <f t="shared" si="0"/>
         <v>71.878504672897193</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47">
+    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C47">
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
-      <c r="B47">
+      <c r="D47">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="C47">
+      <c r="E47">
         <f t="shared" si="0"/>
         <v>73.020768431983385</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48">
+    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C48">
         <f t="shared" si="1"/>
         <v>87.8</v>
       </c>
-      <c r="B48">
+      <c r="D48">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="C48">
+      <c r="E48">
         <f t="shared" si="0"/>
         <v>74.163032191069576</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49">
+    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C49">
         <f t="shared" si="1"/>
         <v>89.6</v>
       </c>
-      <c r="B49">
+      <c r="D49">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="C49">
+      <c r="E49">
         <f t="shared" si="0"/>
         <v>75.305295950155767</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50">
+    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C50">
         <f t="shared" si="1"/>
         <v>91.4</v>
       </c>
-      <c r="B50">
+      <c r="D50">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="C50">
+      <c r="E50">
         <f t="shared" si="0"/>
         <v>76.447559709241943</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51">
+    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C51">
         <f t="shared" si="1"/>
         <v>93.2</v>
       </c>
-      <c r="B51">
+      <c r="D51">
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="C51">
+      <c r="E51">
         <f t="shared" si="0"/>
         <v>77.589823468328149</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52">
+    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C52">
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
-      <c r="B52">
+      <c r="D52">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="C52">
+      <c r="E52">
         <f t="shared" si="0"/>
         <v>78.732087227414326</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53">
+    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C53">
         <f t="shared" si="1"/>
         <v>96.8</v>
       </c>
-      <c r="B53">
+      <c r="D53">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="C53">
+      <c r="E53">
         <f t="shared" si="0"/>
         <v>79.874350986500517</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54">
+    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C54">
         <f t="shared" si="1"/>
         <v>98.6</v>
       </c>
-      <c r="B54">
+      <c r="D54">
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="C54">
+      <c r="E54">
         <f t="shared" si="0"/>
         <v>81.016614745586708</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55">
+    <row r="55" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C55">
         <f t="shared" si="1"/>
         <v>100.4</v>
       </c>
-      <c r="B55">
+      <c r="D55">
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="C55">
+      <c r="E55">
         <f t="shared" si="0"/>
         <v>82.158878504672899</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56">
+    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C56">
         <f t="shared" si="1"/>
         <v>102.2</v>
       </c>
-      <c r="B56">
+      <c r="D56">
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="C56">
+      <c r="E56">
         <f t="shared" si="0"/>
         <v>83.30114226375909</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57">
+    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C57">
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
-      <c r="B57">
+      <c r="D57">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="C57">
+      <c r="E57">
         <f t="shared" si="0"/>
         <v>84.443406022845267</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58">
+    <row r="58" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C58">
         <f t="shared" si="1"/>
         <v>105.8</v>
       </c>
-      <c r="B58">
+      <c r="D58">
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="C58">
+      <c r="E58">
         <f t="shared" si="0"/>
         <v>85.585669781931472</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59">
+    <row r="59" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C59">
         <f t="shared" si="1"/>
         <v>107.6</v>
       </c>
-      <c r="B59">
+      <c r="D59">
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="C59">
+      <c r="E59">
         <f t="shared" si="0"/>
         <v>86.727933541017649</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60">
+    <row r="60" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C60">
         <f t="shared" si="1"/>
         <v>109.4</v>
       </c>
-      <c r="B60">
+      <c r="D60">
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="C60">
+      <c r="E60">
         <f t="shared" si="0"/>
         <v>87.87019730010384</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61">
+    <row r="61" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C61">
         <f t="shared" si="1"/>
         <v>111.2</v>
       </c>
-      <c r="B61">
+      <c r="D61">
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="C61">
+      <c r="E61">
         <f t="shared" si="0"/>
         <v>89.012461059190031</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62">
+    <row r="62" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C62">
         <f t="shared" si="1"/>
         <v>113</v>
       </c>
-      <c r="B62">
+      <c r="D62">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="C62">
+      <c r="E62">
         <f t="shared" si="0"/>
         <v>90.154724818276222</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
+    <row r="65" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A66" s="1"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B66" s="4"/>
-      <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="4"/>
-      <c r="G66" s="4"/>
-      <c r="H66" s="4"/>
-      <c r="I66" s="4"/>
-      <c r="J66" s="4"/>
-      <c r="K66" s="4"/>
-      <c r="L66" s="4"/>
-      <c r="M66" s="4"/>
-      <c r="N66" s="4"/>
-      <c r="O66" s="4"/>
-      <c r="P66" s="5"/>
-    </row>
-    <row r="67" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="6"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="7"/>
-      <c r="D67" s="7"/>
-      <c r="E67" s="7"/>
-      <c r="F67" s="7"/>
-      <c r="G67" s="7"/>
-      <c r="H67" s="7"/>
-      <c r="I67" s="7"/>
-      <c r="J67" s="7"/>
-      <c r="K67" s="7"/>
-      <c r="L67" s="7"/>
-      <c r="M67" s="7"/>
-      <c r="N67" s="7"/>
-      <c r="O67" s="7"/>
-      <c r="P67" s="8"/>
-    </row>
-    <row r="68" spans="1:16" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="9" t="s">
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J66" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K66" s="2"/>
+      <c r="L66" s="2"/>
+      <c r="M66" s="2"/>
+      <c r="N66" s="2"/>
+      <c r="O66" s="2"/>
+      <c r="P66" s="2"/>
+      <c r="Q66" s="2"/>
+      <c r="R66" s="3"/>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A67" s="4"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="5">
+        <v>1.9</v>
+      </c>
+      <c r="J67" s="5">
+        <v>16.5</v>
+      </c>
+      <c r="K67" s="5"/>
+      <c r="L67" s="5"/>
+      <c r="M67" s="5"/>
+      <c r="N67" s="5"/>
+      <c r="O67" s="5"/>
+      <c r="P67" s="5"/>
+      <c r="Q67" s="5"/>
+      <c r="R67" s="6"/>
+    </row>
+    <row r="68" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C68" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="D68" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="E68" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F68" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="G68" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="H68" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F68" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G68" s="7"/>
-      <c r="H68" s="7"/>
-      <c r="I68" s="7"/>
-      <c r="J68" s="7"/>
-      <c r="K68" s="7"/>
-      <c r="L68" s="7"/>
-      <c r="M68" s="7"/>
-      <c r="N68" s="7"/>
-      <c r="O68" s="7"/>
-      <c r="P68" s="8"/>
-    </row>
-    <row r="69" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="10">
+      <c r="I68" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J68" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="K68" s="5"/>
+      <c r="L68" s="5"/>
+      <c r="M68" s="5"/>
+      <c r="N68" s="5"/>
+      <c r="O68" s="5"/>
+      <c r="P68" s="5"/>
+      <c r="Q68" s="5"/>
+      <c r="R68" s="6"/>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A69" s="12">
+        <v>45279</v>
+      </c>
+      <c r="B69" s="8"/>
+      <c r="C69" s="8">
         <v>28</v>
       </c>
-      <c r="B69" s="2">
+      <c r="D69" s="10">
         <v>-9</v>
       </c>
-      <c r="C69" s="2">
+      <c r="E69" s="5">
+        <f>(D69*9/5)+32</f>
         <v>15.8</v>
       </c>
-      <c r="D69" s="2">
+      <c r="F69" s="10">
         <v>-3</v>
       </c>
-      <c r="E69" s="2">
+      <c r="G69" s="8">
         <v>-12</v>
       </c>
-      <c r="F69" s="2">
+      <c r="H69" s="8">
         <v>-4</v>
       </c>
-      <c r="G69" s="7"/>
-      <c r="H69" s="7"/>
-      <c r="I69" s="7"/>
-      <c r="J69" s="7"/>
-      <c r="K69" s="7"/>
-      <c r="L69" s="7"/>
-      <c r="M69" s="7"/>
-      <c r="N69" s="7"/>
-      <c r="O69" s="7"/>
-      <c r="P69" s="8"/>
-    </row>
-    <row r="70" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="10">
+      <c r="I69" s="5">
+        <f>(D69*$I$67)+$J$67</f>
+        <v>-0.59999999999999787</v>
+      </c>
+      <c r="J69" s="5">
+        <f>I69-F69</f>
+        <v>2.4000000000000021</v>
+      </c>
+      <c r="K69" s="5"/>
+      <c r="L69" s="5"/>
+      <c r="M69" s="5"/>
+      <c r="N69" s="5"/>
+      <c r="O69" s="5"/>
+      <c r="P69" s="5"/>
+      <c r="Q69" s="5"/>
+      <c r="R69" s="6"/>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A70" s="12">
+        <v>45279</v>
+      </c>
+      <c r="B70" s="8"/>
+      <c r="C70" s="8">
         <v>45</v>
       </c>
-      <c r="B70" s="2">
+      <c r="D70" s="10">
         <v>5.6</v>
       </c>
-      <c r="C70" s="2">
+      <c r="E70" s="5">
+        <f>(D70*9/5)+32</f>
         <v>42.08</v>
       </c>
-      <c r="D70" s="2">
+      <c r="F70" s="10">
         <v>20</v>
       </c>
-      <c r="E70" s="2">
+      <c r="G70" s="8">
         <v>28</v>
       </c>
-      <c r="F70" s="2">
+      <c r="H70" s="8">
         <v>22</v>
       </c>
-      <c r="G70" s="7"/>
-      <c r="H70" s="7"/>
-      <c r="I70" s="7"/>
-      <c r="J70" s="7"/>
-      <c r="K70" s="7"/>
-      <c r="L70" s="7"/>
-      <c r="M70" s="7"/>
-      <c r="N70" s="7"/>
-      <c r="O70" s="7"/>
-      <c r="P70" s="8"/>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A71" s="6"/>
-      <c r="B71" s="7"/>
-      <c r="C71" s="7"/>
-      <c r="D71" s="7"/>
-      <c r="E71" s="7"/>
-      <c r="F71" s="7"/>
-      <c r="G71" s="7"/>
-      <c r="H71" s="7"/>
-      <c r="I71" s="7"/>
-      <c r="J71" s="7"/>
-      <c r="K71" s="7"/>
-      <c r="L71" s="7"/>
-      <c r="M71" s="7"/>
-      <c r="N71" s="7"/>
-      <c r="O71" s="7"/>
-      <c r="P71" s="8"/>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A72" s="6"/>
-      <c r="B72" s="7"/>
-      <c r="C72" s="7"/>
-      <c r="D72" s="7"/>
-      <c r="E72" s="7"/>
-      <c r="F72" s="7"/>
-      <c r="G72" s="7"/>
-      <c r="H72" s="7"/>
-      <c r="I72" s="7"/>
-      <c r="J72" s="7"/>
-      <c r="K72" s="7"/>
-      <c r="L72" s="7"/>
-      <c r="M72" s="7"/>
-      <c r="N72" s="7"/>
-      <c r="O72" s="7"/>
-      <c r="P72" s="8"/>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A73" s="6"/>
-      <c r="B73" s="7"/>
-      <c r="C73" s="7"/>
-      <c r="D73" s="7"/>
-      <c r="E73" s="7"/>
-      <c r="F73" s="7"/>
-      <c r="G73" s="7"/>
-      <c r="H73" s="7"/>
-      <c r="I73" s="7"/>
-      <c r="J73" s="7"/>
-      <c r="K73" s="7"/>
-      <c r="L73" s="7"/>
-      <c r="M73" s="7"/>
-      <c r="N73" s="7"/>
-      <c r="O73" s="7"/>
-      <c r="P73" s="8"/>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A74" s="6"/>
-      <c r="B74" s="7"/>
-      <c r="C74" s="7"/>
-      <c r="D74" s="7"/>
-      <c r="E74" s="7"/>
-      <c r="F74" s="7"/>
-      <c r="G74" s="7"/>
-      <c r="H74" s="7"/>
-      <c r="I74" s="7"/>
-      <c r="J74" s="7"/>
-      <c r="K74" s="7"/>
-      <c r="L74" s="7"/>
-      <c r="M74" s="7"/>
-      <c r="N74" s="7"/>
-      <c r="O74" s="7"/>
-      <c r="P74" s="8"/>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A75" s="6"/>
-      <c r="B75" s="7"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="7"/>
-      <c r="E75" s="7"/>
-      <c r="F75" s="7"/>
-      <c r="G75" s="7"/>
-      <c r="H75" s="7"/>
-      <c r="I75" s="7"/>
-      <c r="J75" s="7"/>
-      <c r="K75" s="7"/>
-      <c r="L75" s="7"/>
-      <c r="M75" s="7"/>
-      <c r="N75" s="7"/>
-      <c r="O75" s="7"/>
-      <c r="P75" s="8"/>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A76" s="6"/>
-      <c r="B76" s="7"/>
-      <c r="C76" s="7"/>
-      <c r="D76" s="7"/>
-      <c r="E76" s="7"/>
-      <c r="F76" s="7"/>
-      <c r="G76" s="7"/>
-      <c r="H76" s="7"/>
-      <c r="I76" s="7"/>
-      <c r="J76" s="7"/>
-      <c r="K76" s="7"/>
-      <c r="L76" s="7"/>
-      <c r="M76" s="7"/>
-      <c r="N76" s="7"/>
-      <c r="O76" s="7"/>
-      <c r="P76" s="8"/>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A77" s="6"/>
-      <c r="B77" s="7"/>
-      <c r="C77" s="7"/>
-      <c r="D77" s="7"/>
-      <c r="E77" s="7"/>
-      <c r="F77" s="7"/>
-      <c r="G77" s="7"/>
-      <c r="H77" s="7"/>
-      <c r="I77" s="7"/>
-      <c r="J77" s="7"/>
-      <c r="K77" s="7"/>
-      <c r="L77" s="7"/>
-      <c r="M77" s="7"/>
-      <c r="N77" s="7"/>
-      <c r="O77" s="7"/>
-      <c r="P77" s="8"/>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A78" s="6"/>
-      <c r="B78" s="7"/>
-      <c r="C78" s="7"/>
-      <c r="D78" s="7"/>
-      <c r="E78" s="7"/>
-      <c r="F78" s="7"/>
-      <c r="G78" s="7"/>
-      <c r="H78" s="7"/>
-      <c r="I78" s="7"/>
-      <c r="J78" s="7"/>
-      <c r="K78" s="7"/>
-      <c r="L78" s="7"/>
-      <c r="M78" s="7"/>
-      <c r="N78" s="7"/>
-      <c r="O78" s="7"/>
-      <c r="P78" s="8"/>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G79" s="7"/>
-      <c r="H79" s="7"/>
-      <c r="I79" s="7"/>
-      <c r="J79" s="7"/>
-      <c r="K79" s="7"/>
-      <c r="L79" s="7"/>
-      <c r="M79" s="7"/>
-      <c r="N79" s="7"/>
-      <c r="O79" s="7"/>
-      <c r="P79" s="8"/>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A80" s="6"/>
-      <c r="B80" s="7"/>
-      <c r="C80" s="7"/>
-      <c r="D80" s="7"/>
-      <c r="E80" s="7"/>
-      <c r="F80" s="7"/>
-      <c r="G80" s="7"/>
-      <c r="H80" s="7"/>
-      <c r="I80" s="7"/>
-      <c r="J80" s="7"/>
-      <c r="K80" s="7"/>
-      <c r="L80" s="7"/>
-      <c r="M80" s="7"/>
-      <c r="N80" s="7"/>
-      <c r="O80" s="7"/>
-      <c r="P80" s="8"/>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A81" s="6"/>
-      <c r="B81" s="7"/>
-      <c r="C81" s="7"/>
-      <c r="D81" s="7"/>
-      <c r="E81" s="7"/>
-      <c r="F81" s="7"/>
-      <c r="G81" s="7"/>
-      <c r="H81" s="7"/>
-      <c r="I81" s="7"/>
-      <c r="J81" s="7"/>
-      <c r="K81" s="7"/>
-      <c r="L81" s="7"/>
-      <c r="M81" s="7"/>
-      <c r="N81" s="7"/>
-      <c r="O81" s="7"/>
-      <c r="P81" s="8"/>
-    </row>
-    <row r="82" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="11"/>
-      <c r="B82" s="12"/>
-      <c r="C82" s="12"/>
-      <c r="D82" s="12"/>
-      <c r="E82" s="12"/>
-      <c r="F82" s="12"/>
-      <c r="G82" s="12"/>
-      <c r="H82" s="12"/>
-      <c r="I82" s="12"/>
-      <c r="J82" s="12"/>
-      <c r="K82" s="12"/>
-      <c r="L82" s="12"/>
-      <c r="M82" s="12"/>
-      <c r="N82" s="12"/>
-      <c r="O82" s="12"/>
-      <c r="P82" s="13"/>
+      <c r="I70" s="5">
+        <f>(D70*$I$67)+$J$67</f>
+        <v>27.14</v>
+      </c>
+      <c r="J70" s="5">
+        <f>I70-F70</f>
+        <v>7.1400000000000006</v>
+      </c>
+      <c r="K70" s="5"/>
+      <c r="L70" s="5"/>
+      <c r="M70" s="5"/>
+      <c r="N70" s="5"/>
+      <c r="O70" s="5"/>
+      <c r="P70" s="5"/>
+      <c r="Q70" s="5"/>
+      <c r="R70" s="6"/>
+      <c r="U70" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A71" s="12">
+        <v>45280</v>
+      </c>
+      <c r="B71" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C71" s="5"/>
+      <c r="D71" s="11">
+        <v>25.31</v>
+      </c>
+      <c r="E71" s="5">
+        <f>(D71*9/5)+32</f>
+        <v>77.557999999999993</v>
+      </c>
+      <c r="F71" s="11">
+        <v>70.7</v>
+      </c>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="5">
+        <f>(D71*$I$67)+$J$67</f>
+        <v>64.588999999999999</v>
+      </c>
+      <c r="J71" s="5">
+        <f>I71-F71</f>
+        <v>-6.1110000000000042</v>
+      </c>
+      <c r="K71" s="5"/>
+      <c r="L71" s="5"/>
+      <c r="M71" s="5"/>
+      <c r="N71" s="5"/>
+      <c r="O71" s="5"/>
+      <c r="P71" s="5"/>
+      <c r="Q71" s="5"/>
+      <c r="R71" s="6"/>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A72" s="12">
+        <v>45281</v>
+      </c>
+      <c r="B72" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C72" s="5"/>
+      <c r="D72" s="11">
+        <v>9.8478999999999992</v>
+      </c>
+      <c r="E72" s="5">
+        <f>(D72*9/5)+32</f>
+        <v>49.726219999999998</v>
+      </c>
+      <c r="F72" s="11">
+        <v>41.5</v>
+      </c>
+      <c r="G72" s="5"/>
+      <c r="H72" s="5"/>
+      <c r="I72" s="5">
+        <f>(D72*$I$67)+$J$67</f>
+        <v>35.211010000000002</v>
+      </c>
+      <c r="J72" s="5">
+        <f>I72-F72</f>
+        <v>-6.2889899999999983</v>
+      </c>
+      <c r="K72" s="5"/>
+      <c r="L72" s="5"/>
+      <c r="M72" s="5"/>
+      <c r="N72" s="5"/>
+      <c r="O72" s="5"/>
+      <c r="P72" s="5"/>
+      <c r="Q72" s="5"/>
+      <c r="R72" s="6"/>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A73" s="12">
+        <v>45281</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C73" s="5"/>
+      <c r="D73" s="11">
+        <v>10.08</v>
+      </c>
+      <c r="E73" s="5">
+        <f>(D73*9/5)+32</f>
+        <v>50.143999999999998</v>
+      </c>
+      <c r="F73" s="11">
+        <v>43</v>
+      </c>
+      <c r="G73" s="5"/>
+      <c r="H73" s="5"/>
+      <c r="I73" s="5">
+        <f>(D73*$I$67)+$J$67</f>
+        <v>35.652000000000001</v>
+      </c>
+      <c r="J73" s="5">
+        <f>I73-F73</f>
+        <v>-7.347999999999999</v>
+      </c>
+      <c r="K73" s="5"/>
+      <c r="L73" s="5"/>
+      <c r="M73" s="5"/>
+      <c r="N73" s="5"/>
+      <c r="O73" s="5"/>
+      <c r="P73" s="5"/>
+      <c r="Q73" s="5"/>
+      <c r="R73" s="6"/>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A74" s="12">
+        <v>45281</v>
+      </c>
+      <c r="B74" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C74" s="5"/>
+      <c r="D74" s="11">
+        <v>8.6370000000000005</v>
+      </c>
+      <c r="E74" s="13">
+        <f>(D74*9/5)+32</f>
+        <v>47.546599999999998</v>
+      </c>
+      <c r="F74" s="11">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="G74" s="5"/>
+      <c r="H74" s="5"/>
+      <c r="I74" s="5">
+        <f>(D74*$I$67)+$J$67</f>
+        <v>32.910299999999999</v>
+      </c>
+      <c r="J74" s="5">
+        <f>I74-F74</f>
+        <v>-7.8896999999999977</v>
+      </c>
+      <c r="K74" s="5"/>
+      <c r="L74" s="5"/>
+      <c r="M74" s="5"/>
+      <c r="N74" s="5"/>
+      <c r="O74" s="5"/>
+      <c r="P74" s="5"/>
+      <c r="Q74" s="5"/>
+      <c r="R74" s="6"/>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A75" s="12">
+        <v>45282</v>
+      </c>
+      <c r="B75" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C75" s="5"/>
+      <c r="D75" s="11">
+        <v>14.8734</v>
+      </c>
+      <c r="E75" s="13">
+        <f>(D75*9/5)+32</f>
+        <v>58.772120000000001</v>
+      </c>
+      <c r="F75" s="11">
+        <v>45.9</v>
+      </c>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
+      <c r="I75" s="5">
+        <f>(D75*$I$67)+$J$67</f>
+        <v>44.759460000000004</v>
+      </c>
+      <c r="J75" s="5">
+        <f>I75-F75</f>
+        <v>-1.1405399999999943</v>
+      </c>
+      <c r="K75" s="5"/>
+      <c r="L75" s="5"/>
+      <c r="M75" s="5"/>
+      <c r="N75" s="5"/>
+      <c r="O75" s="5"/>
+      <c r="P75" s="5"/>
+      <c r="Q75" s="5"/>
+      <c r="R75" s="6"/>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A76" s="12">
+        <v>45282</v>
+      </c>
+      <c r="B76" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C76" s="5"/>
+      <c r="D76" s="11">
+        <v>15.1111</v>
+      </c>
+      <c r="E76" s="13">
+        <f>(D76*9/5)+32</f>
+        <v>59.199979999999996</v>
+      </c>
+      <c r="F76" s="11">
+        <v>46.8</v>
+      </c>
+      <c r="G76" s="5"/>
+      <c r="H76" s="5"/>
+      <c r="I76" s="5">
+        <f>(D76*$I$67)+$J$67</f>
+        <v>45.211089999999999</v>
+      </c>
+      <c r="J76" s="5">
+        <f>I76-F76</f>
+        <v>-1.5889099999999985</v>
+      </c>
+      <c r="K76" s="5"/>
+      <c r="L76" s="5"/>
+      <c r="M76" s="5"/>
+      <c r="N76" s="5"/>
+      <c r="O76" s="5"/>
+      <c r="P76" s="5"/>
+      <c r="Q76" s="5"/>
+      <c r="R76" s="6"/>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A77" s="12">
+        <v>45282</v>
+      </c>
+      <c r="B77" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C77" s="5"/>
+      <c r="D77" s="11">
+        <v>16.757100000000001</v>
+      </c>
+      <c r="E77" s="13">
+        <f>(D77*9/5)+32</f>
+        <v>62.162780000000005</v>
+      </c>
+      <c r="F77" s="11">
+        <v>49.6</v>
+      </c>
+      <c r="G77" s="5"/>
+      <c r="H77" s="5"/>
+      <c r="I77" s="5">
+        <f>(D77*$I$67)+$J$67</f>
+        <v>48.33849</v>
+      </c>
+      <c r="J77" s="5">
+        <f>I77-F77</f>
+        <v>-1.2615100000000012</v>
+      </c>
+      <c r="K77" s="5"/>
+      <c r="L77" s="5"/>
+      <c r="M77" s="5"/>
+      <c r="N77" s="5"/>
+      <c r="O77" s="5"/>
+      <c r="P77" s="5"/>
+      <c r="Q77" s="5"/>
+      <c r="R77" s="6"/>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A78" s="12">
+        <v>45282</v>
+      </c>
+      <c r="B78" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C78" s="5"/>
+      <c r="D78" s="11">
+        <v>17.616599999999998</v>
+      </c>
+      <c r="E78" s="13">
+        <f>(D78*9/5)+32</f>
+        <v>63.709879999999998</v>
+      </c>
+      <c r="F78" s="11">
+        <v>50</v>
+      </c>
+      <c r="G78" s="5"/>
+      <c r="H78" s="5"/>
+      <c r="I78" s="5">
+        <f>(D78*$I$67)+$J$67</f>
+        <v>49.971539999999997</v>
+      </c>
+      <c r="J78" s="5">
+        <f>I78-F78</f>
+        <v>-2.8460000000002594E-2</v>
+      </c>
+      <c r="K78" s="5"/>
+      <c r="L78" s="5"/>
+      <c r="M78" s="5"/>
+      <c r="N78" s="5"/>
+      <c r="O78" s="5"/>
+      <c r="P78" s="5"/>
+      <c r="Q78" s="5"/>
+      <c r="R78" s="6"/>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A79" s="12">
+        <v>45282</v>
+      </c>
+      <c r="B79" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C79" s="5"/>
+      <c r="D79" s="11">
+        <v>19.024799999999999</v>
+      </c>
+      <c r="E79" s="13">
+        <f>(D79*9/5)+32</f>
+        <v>66.244640000000004</v>
+      </c>
+      <c r="F79" s="11">
+        <v>52.3</v>
+      </c>
+      <c r="G79" s="5"/>
+      <c r="H79" s="5"/>
+      <c r="I79" s="5">
+        <f>(D79*$I$67)+$J$67</f>
+        <v>52.647119999999994</v>
+      </c>
+      <c r="J79" s="5">
+        <f>I79-F79</f>
+        <v>0.34711999999999676</v>
+      </c>
+      <c r="K79" s="5"/>
+      <c r="L79" s="5"/>
+      <c r="M79" s="5"/>
+      <c r="N79" s="5"/>
+      <c r="O79" s="5"/>
+      <c r="P79" s="5"/>
+      <c r="Q79" s="5"/>
+      <c r="R79" s="6"/>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A80" s="12">
+        <v>45282</v>
+      </c>
+      <c r="B80" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C80" s="5"/>
+      <c r="D80" s="11">
+        <v>19.481999999999999</v>
+      </c>
+      <c r="E80" s="13">
+        <f>(D80*9/5)+32</f>
+        <v>67.067599999999999</v>
+      </c>
+      <c r="F80" s="11">
+        <v>53.22</v>
+      </c>
+      <c r="G80" s="5"/>
+      <c r="H80" s="5"/>
+      <c r="I80" s="5">
+        <f>(D80*$I$67)+$J$67</f>
+        <v>53.515799999999999</v>
+      </c>
+      <c r="J80" s="5">
+        <f>I80-F80</f>
+        <v>0.29579999999999984</v>
+      </c>
+      <c r="K80" s="5"/>
+      <c r="L80" s="5"/>
+      <c r="M80" s="5"/>
+      <c r="N80" s="5"/>
+      <c r="O80" s="5"/>
+      <c r="P80" s="5"/>
+      <c r="Q80" s="5"/>
+      <c r="R80" s="6"/>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A81" s="12">
+        <v>45282</v>
+      </c>
+      <c r="B81" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C81" s="5"/>
+      <c r="D81" s="11">
+        <v>20.1587</v>
+      </c>
+      <c r="E81" s="13">
+        <f>(D81*9/5)+32</f>
+        <v>68.285660000000007</v>
+      </c>
+      <c r="F81" s="11">
+        <v>54</v>
+      </c>
+      <c r="G81" s="5"/>
+      <c r="H81" s="5"/>
+      <c r="I81" s="5">
+        <f>(D81*$I$67)+$J$67</f>
+        <v>54.80153</v>
+      </c>
+      <c r="J81" s="5">
+        <f>I81-F81</f>
+        <v>0.80152999999999963</v>
+      </c>
+      <c r="K81" s="5"/>
+      <c r="L81" s="5"/>
+      <c r="M81" s="5"/>
+      <c r="N81" s="5"/>
+      <c r="O81" s="5"/>
+      <c r="P81" s="5"/>
+      <c r="Q81" s="5"/>
+      <c r="R81" s="6"/>
+    </row>
+    <row r="82" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="19">
+        <v>45282</v>
+      </c>
+      <c r="B82" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D82" s="11">
+        <v>20.7439</v>
+      </c>
+      <c r="E82" s="13">
+        <f>(D82*9/5)+32</f>
+        <v>69.339020000000005</v>
+      </c>
+      <c r="F82" s="11">
+        <v>55</v>
+      </c>
+      <c r="I82" s="5">
+        <f>(D82*$I$67)+$J$67</f>
+        <v>55.913409999999999</v>
+      </c>
+      <c r="J82" s="5">
+        <f>I82-F82</f>
+        <v>0.91340999999999894</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A83" s="12">
+        <v>45282</v>
+      </c>
+      <c r="B83" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D83" s="11">
+        <v>20.160299999999999</v>
+      </c>
+      <c r="E83" s="13">
+        <f>(D83*9/5)+32</f>
+        <v>68.288539999999998</v>
+      </c>
+      <c r="F83" s="11">
+        <v>56.8</v>
+      </c>
+      <c r="I83" s="5">
+        <f>(D83*$I$67)+$J$67</f>
+        <v>54.804569999999998</v>
+      </c>
+      <c r="J83" s="5">
+        <f>I83-F83</f>
+        <v>-1.9954299999999989</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A84" s="12">
+        <v>45282</v>
+      </c>
+      <c r="B84" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D84" s="11">
+        <v>21.7681</v>
+      </c>
+      <c r="E84" s="13">
+        <f>(D84*9/5)+32</f>
+        <v>71.182580000000002</v>
+      </c>
+      <c r="F84" s="11">
+        <v>57</v>
+      </c>
+      <c r="I84" s="5">
+        <f>(D84*$I$67)+$J$67</f>
+        <v>57.859389999999998</v>
+      </c>
+      <c r="J84" s="5">
+        <f>I84-F84</f>
+        <v>0.85938999999999766</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A85" s="12">
+        <v>45282</v>
+      </c>
+      <c r="B85" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D85" s="11">
+        <v>22.389900000000001</v>
+      </c>
+      <c r="E85" s="13">
+        <f>(D85*9/5)+32</f>
+        <v>72.301820000000006</v>
+      </c>
+      <c r="F85" s="11">
+        <v>58.1</v>
+      </c>
+      <c r="I85" s="5">
+        <f>(D85*$I$67)+$J$67</f>
+        <v>59.04081</v>
+      </c>
+      <c r="J85" s="5">
+        <f>I85-F85</f>
+        <v>0.94080999999999904</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A86" s="12">
+        <v>45282</v>
+      </c>
+      <c r="B86" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D86" s="11">
+        <v>22.956800000000001</v>
+      </c>
+      <c r="E86" s="13">
+        <f>(D86*9/5)+32</f>
+        <v>73.322239999999994</v>
+      </c>
+      <c r="F86" s="11">
+        <v>59.4</v>
+      </c>
+      <c r="I86" s="5">
+        <f>(D86*$I$67)+$J$67</f>
+        <v>60.117919999999998</v>
+      </c>
+      <c r="J86" s="5">
+        <f>I86-F86</f>
+        <v>0.71791999999999945</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A87" s="12">
+        <v>45282</v>
+      </c>
+      <c r="B87" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D87" s="11">
+        <v>23.340900000000001</v>
+      </c>
+      <c r="E87" s="13">
+        <f>(D87*9/5)+32</f>
+        <v>74.013620000000003</v>
+      </c>
+      <c r="F87" s="11">
+        <v>60.3</v>
+      </c>
+      <c r="I87" s="5">
+        <f>(D87*$I$67)+$J$67</f>
+        <v>60.847709999999999</v>
+      </c>
+      <c r="J87" s="5">
+        <f>I87-F87</f>
+        <v>0.54771000000000214</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A88" s="12">
+        <v>45282</v>
+      </c>
+      <c r="B88" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D88" s="11">
+        <v>23.889500000000002</v>
+      </c>
+      <c r="E88" s="13">
+        <f>(D88*9/5)+32</f>
+        <v>75.001100000000008</v>
+      </c>
+      <c r="F88" s="11">
+        <v>61</v>
+      </c>
+      <c r="I88" s="5">
+        <f>(D88*$I$67)+$J$67</f>
+        <v>61.890050000000002</v>
+      </c>
+      <c r="J88" s="5">
+        <f>I88-F88</f>
+        <v>0.89005000000000223</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A89" s="12">
+        <v>45282</v>
+      </c>
+      <c r="B89" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D89" s="11">
+        <v>24.346699999999998</v>
+      </c>
+      <c r="E89" s="13">
+        <f>(D89*9/5)+32</f>
+        <v>75.824060000000003</v>
+      </c>
+      <c r="F89" s="11">
+        <v>62.2</v>
+      </c>
+      <c r="I89" s="5">
+        <f>(D89*$I$67)+$J$67</f>
+        <v>62.758729999999993</v>
+      </c>
+      <c r="J89" s="5">
+        <f>I89-F89</f>
+        <v>0.55872999999998996</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A90" s="12">
+        <v>45282</v>
+      </c>
+      <c r="B90" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D90" s="11">
+        <v>24.803899999999999</v>
+      </c>
+      <c r="E90" s="13">
+        <f>(D90*9/5)+32</f>
+        <v>76.647019999999998</v>
+      </c>
+      <c r="F90" s="11">
+        <v>63</v>
+      </c>
+      <c r="I90" s="5">
+        <f>(D90*$I$67)+$J$67</f>
+        <v>63.627409999999998</v>
+      </c>
+      <c r="J90" s="5">
+        <f>I90-F90</f>
+        <v>0.62740999999999758</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A91" s="12">
+        <v>45282</v>
+      </c>
+      <c r="B91" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D91" s="11">
+        <v>25.242799999999999</v>
+      </c>
+      <c r="E91" s="13">
+        <f>(D91*9/5)+32</f>
+        <v>77.437039999999996</v>
+      </c>
+      <c r="F91" s="11">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="I91" s="5">
+        <f>(D91*$I$67)+$J$67</f>
+        <v>64.461320000000001</v>
+      </c>
+      <c r="J91" s="5">
+        <f>I91-F91</f>
+        <v>-0.1386799999999937</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A92" s="12">
+        <v>45282</v>
+      </c>
+      <c r="B92" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D92" s="11">
+        <v>25.809799999999999</v>
+      </c>
+      <c r="E92" s="13">
+        <f>(D92*9/5)+32</f>
+        <v>78.457639999999998</v>
+      </c>
+      <c r="F92" s="11">
+        <v>65.3</v>
+      </c>
+      <c r="I92" s="5">
+        <f>(D92*$I$67)+$J$67</f>
+        <v>65.538619999999995</v>
+      </c>
+      <c r="J92" s="5">
+        <f>I92-F92</f>
+        <v>0.23861999999999739</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A93" s="12">
+        <v>45282</v>
+      </c>
+      <c r="B93" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D93" s="11">
+        <v>26.285299999999999</v>
+      </c>
+      <c r="E93" s="13">
+        <f>(D93*9/5)+32</f>
+        <v>79.313540000000003</v>
+      </c>
+      <c r="F93" s="11">
+        <v>66.2</v>
+      </c>
+      <c r="I93" s="5">
+        <f>(D93*$I$67)+$J$67</f>
+        <v>66.442070000000001</v>
+      </c>
+      <c r="J93" s="5">
+        <f>I93-F93</f>
+        <v>0.24206999999999823</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A94" s="12">
+        <v>45282</v>
+      </c>
+      <c r="B94" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D94" s="11">
+        <v>26.8705</v>
+      </c>
+      <c r="E94" s="13">
+        <f>(D94*9/5)+32</f>
+        <v>80.366900000000001</v>
+      </c>
+      <c r="F94" s="11">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="I94" s="5">
+        <f>(D94*$I$67)+$J$67</f>
+        <v>67.55395</v>
+      </c>
+      <c r="J94" s="5">
+        <f>I94-F94</f>
+        <v>0.45395000000000607</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A95" s="12">
+        <v>45282</v>
+      </c>
+      <c r="B95" t="s">
+        <v>43</v>
+      </c>
+      <c r="D95" s="11">
+        <v>28.333600000000001</v>
+      </c>
+      <c r="E95" s="13">
+        <f>(D95*9/5)+32</f>
+        <v>83.000479999999996</v>
+      </c>
+      <c r="F95" s="11">
+        <v>70.7</v>
+      </c>
+      <c r="I95" s="5">
+        <f>(D95*$I$67)+$J$67</f>
+        <v>70.333839999999995</v>
+      </c>
+      <c r="J95" s="5">
+        <f>I95-F95</f>
+        <v>-0.36616000000000781</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A96" s="12">
+        <v>45282</v>
+      </c>
+      <c r="B96" t="s">
+        <v>45</v>
+      </c>
+      <c r="D96" s="11">
+        <v>28.553000000000001</v>
+      </c>
+      <c r="E96" s="13">
+        <f>(D96*9/5)+32</f>
+        <v>83.395400000000009</v>
+      </c>
+      <c r="F96" s="11">
+        <v>71</v>
+      </c>
+      <c r="I96" s="5">
+        <f>(D96*$I$67)+$J$67</f>
+        <v>70.750699999999995</v>
+      </c>
+      <c r="J96" s="13">
+        <f>I96-F96</f>
+        <v>-0.24930000000000518</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" s="12">
+        <v>45282</v>
+      </c>
+      <c r="B97" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D97" s="11">
+        <v>29.211400000000001</v>
+      </c>
+      <c r="E97" s="13">
+        <f>(D97*9/5)+32</f>
+        <v>84.580520000000007</v>
+      </c>
+      <c r="F97" s="11">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="I97" s="5">
+        <f>(D97*$I$67)+$J$67</f>
+        <v>72.001660000000001</v>
+      </c>
+      <c r="J97" s="13">
+        <f>I97-F97</f>
+        <v>-9.8339999999993211E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A98" s="12">
+        <v>45282</v>
+      </c>
+      <c r="B98" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D98" s="11">
+        <v>29.430900000000001</v>
+      </c>
+      <c r="E98" s="13">
+        <f>(D98*9/5)+32</f>
+        <v>84.975620000000006</v>
+      </c>
+      <c r="F98" s="11">
+        <v>73</v>
+      </c>
+      <c r="I98" s="5">
+        <f>(D98*$I$67)+$J$67</f>
+        <v>72.418710000000004</v>
+      </c>
+      <c r="J98" s="13">
+        <f>I98-F98</f>
+        <v>-0.58128999999999564</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99" s="12">
+        <v>45282</v>
+      </c>
+      <c r="B99" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D99" s="11">
+        <v>32.667900000000003</v>
+      </c>
+      <c r="E99" s="13">
+        <f>(D99*9/5)+32</f>
+        <v>90.802220000000005</v>
+      </c>
+      <c r="F99" s="11">
+        <v>77.7</v>
+      </c>
+      <c r="I99" s="5">
+        <f>(D99*$I$67)+$J$67</f>
+        <v>78.569010000000006</v>
+      </c>
+      <c r="J99" s="13">
+        <f>I99-F99</f>
+        <v>0.86901000000000295</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100" s="12">
+        <v>45282</v>
+      </c>
+      <c r="B100" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D100" s="11">
+        <v>28.882200000000001</v>
+      </c>
+      <c r="E100" s="13">
+        <f>(D100*9/5)+32</f>
+        <v>83.987960000000001</v>
+      </c>
+      <c r="F100" s="11">
+        <v>76.3</v>
+      </c>
+      <c r="I100" s="5">
+        <f>(D100*$I$67)+$J$67</f>
+        <v>71.376180000000005</v>
+      </c>
+      <c r="J100" s="13">
+        <f>I100-F100</f>
+        <v>-4.9238199999999921</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101" s="19">
+        <v>45284</v>
+      </c>
+      <c r="B101" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D101" s="11">
+        <v>8.3627000000000002</v>
+      </c>
+      <c r="E101" s="13">
+        <f>(D101*9/5)+32</f>
+        <v>47.052860000000003</v>
+      </c>
+      <c r="F101" s="11">
+        <v>38.5</v>
+      </c>
+      <c r="I101" s="5">
+        <f>(D101*$I$67)+$J$67</f>
+        <v>32.389130000000002</v>
+      </c>
+      <c r="J101" s="13">
+        <f>I101-F101</f>
+        <v>-6.1108699999999985</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102" s="19">
+        <v>45284</v>
+      </c>
+      <c r="B102" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D102" s="11">
+        <v>9.5513999999999992</v>
+      </c>
+      <c r="E102" s="13">
+        <f>(D102*9/5)+32</f>
+        <v>49.192520000000002</v>
+      </c>
+      <c r="F102" s="11">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="I102" s="5">
+        <f>(D102*$I$67)+$J$67</f>
+        <v>34.647660000000002</v>
+      </c>
+      <c r="J102" s="13">
+        <f>I102-F102</f>
+        <v>-4.5523400000000009</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103" s="19">
+        <v>45284</v>
+      </c>
+      <c r="B103" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D103" s="11">
+        <v>9.4050999999999991</v>
+      </c>
+      <c r="E103" s="13">
+        <f>(D103*9/5)+32</f>
+        <v>48.929180000000002</v>
+      </c>
+      <c r="F103" s="11">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="I103" s="5">
+        <f>(D103*$I$67)+$J$67</f>
+        <v>34.369689999999999</v>
+      </c>
+      <c r="J103" s="13">
+        <f>I103-F103</f>
+        <v>-5.3303100000000043</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A104" s="19">
+        <v>45284</v>
+      </c>
+      <c r="B104" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D104" s="11">
+        <v>8.4541000000000004</v>
+      </c>
+      <c r="E104" s="13">
+        <f>(D104*9/5)+32</f>
+        <v>47.217379999999999</v>
+      </c>
+      <c r="F104" s="11">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="I104" s="5">
+        <f>(D104*$I$67)+$J$67</f>
+        <v>32.56279</v>
+      </c>
+      <c r="J104" s="13">
+        <f>I104-F104</f>
+        <v>-6.2372099999999975</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A105" s="19">
+        <v>45284</v>
+      </c>
+      <c r="B105" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D105" s="11">
+        <v>9.6611999999999991</v>
+      </c>
+      <c r="E105" s="13">
+        <f>(D105*9/5)+32</f>
+        <v>49.390159999999995</v>
+      </c>
+      <c r="F105" s="11">
+        <v>40.1</v>
+      </c>
+      <c r="I105" s="5">
+        <f>(D105*$I$67)+$J$67</f>
+        <v>34.856279999999998</v>
+      </c>
+      <c r="J105" s="13">
+        <f>I105-F105</f>
+        <v>-5.2437200000000033</v>
+      </c>
+      <c r="K105" s="25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A106" s="19">
+        <v>45284</v>
+      </c>
+      <c r="B106" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D106" s="11">
+        <v>9.5879999999999992</v>
+      </c>
+      <c r="E106" s="13">
+        <f>(D106*9/5)+32</f>
+        <v>49.258399999999995</v>
+      </c>
+      <c r="F106" s="11">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="I106" s="5">
+        <f>(D106*$I$67)+$J$67</f>
+        <v>34.717199999999998</v>
+      </c>
+      <c r="J106" s="13">
+        <f>I106-F106</f>
+        <v>-4.9828000000000046</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A107" s="19">
+        <v>45284</v>
+      </c>
+      <c r="B107" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D107" s="11">
+        <v>10.411</v>
+      </c>
+      <c r="E107" s="13">
+        <f t="shared" ref="E69:E114" si="3">(D107*9/5)+32</f>
+        <v>50.739800000000002</v>
+      </c>
+      <c r="F107" s="11">
+        <v>41.2</v>
+      </c>
+      <c r="I107" s="5">
+        <f t="shared" ref="I70:I114" si="4">(D107*$I$67)+$J$67</f>
+        <v>36.280900000000003</v>
+      </c>
+      <c r="J107" s="13">
+        <f t="shared" ref="J99:J114" si="5">I107-F107</f>
+        <v>-4.9191000000000003</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A108" s="19">
+        <v>45284</v>
+      </c>
+      <c r="B108" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D108" s="11">
+        <v>10.91</v>
+      </c>
+      <c r="E108" s="13">
+        <f t="shared" si="3"/>
+        <v>51.637999999999998</v>
+      </c>
+      <c r="F108" s="11">
+        <v>41.5</v>
+      </c>
+      <c r="I108" s="5">
+        <f t="shared" si="4"/>
+        <v>37.228999999999999</v>
+      </c>
+      <c r="J108" s="13">
+        <f t="shared" si="5"/>
+        <v>-4.2710000000000008</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A109" s="19">
+        <v>45284</v>
+      </c>
+      <c r="B109" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D109" s="11">
+        <v>10.7768</v>
+      </c>
+      <c r="E109" s="13">
+        <f t="shared" si="3"/>
+        <v>51.398240000000001</v>
+      </c>
+      <c r="F109" s="11">
+        <v>41.7</v>
+      </c>
+      <c r="I109" s="13">
+        <f t="shared" si="4"/>
+        <v>36.975920000000002</v>
+      </c>
+      <c r="J109" s="13">
+        <f t="shared" si="5"/>
+        <v>-4.7240800000000007</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A110" s="19">
+        <v>45284</v>
+      </c>
+      <c r="B110" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D110" s="11">
+        <v>10.9779</v>
+      </c>
+      <c r="E110" s="13">
+        <f t="shared" si="3"/>
+        <v>51.760220000000004</v>
+      </c>
+      <c r="F110" s="11">
+        <v>41.7</v>
+      </c>
+      <c r="G110">
+        <v>38</v>
+      </c>
+      <c r="H110">
+        <v>38</v>
+      </c>
+      <c r="I110" s="13">
+        <f t="shared" si="4"/>
+        <v>37.35801</v>
+      </c>
+      <c r="J110" s="13">
+        <f t="shared" si="5"/>
+        <v>-4.3419900000000027</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="20">
+        <v>45284</v>
+      </c>
+      <c r="B111" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D111" s="23">
+        <v>9.33</v>
+      </c>
+      <c r="E111" s="24">
+        <f t="shared" si="3"/>
+        <v>48.793999999999997</v>
+      </c>
+      <c r="F111" s="23">
+        <v>40.5</v>
+      </c>
+      <c r="G111" s="22">
+        <v>31</v>
+      </c>
+      <c r="H111" s="22">
+        <v>34</v>
+      </c>
+      <c r="I111" s="24">
+        <f t="shared" si="4"/>
+        <v>34.227000000000004</v>
+      </c>
+      <c r="J111" s="24">
+        <f t="shared" si="5"/>
+        <v>-6.2729999999999961</v>
+      </c>
+      <c r="K111" s="22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A112" s="19">
+        <v>45284</v>
+      </c>
+      <c r="B112" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D112" s="11">
+        <v>1.37659</v>
+      </c>
+      <c r="E112" s="13">
+        <f t="shared" si="3"/>
+        <v>34.477862000000002</v>
+      </c>
+      <c r="F112" s="11">
+        <v>30.5</v>
+      </c>
+      <c r="G112">
+        <v>24</v>
+      </c>
+      <c r="H112">
+        <v>24</v>
+      </c>
+      <c r="I112" s="13">
+        <f t="shared" si="4"/>
+        <v>19.115521000000001</v>
+      </c>
+      <c r="J112" s="13">
+        <f t="shared" si="5"/>
+        <v>-11.384478999999999</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113" s="19">
+        <v>45284</v>
+      </c>
+      <c r="B113" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D113" s="11">
+        <v>2.0165999999999999</v>
+      </c>
+      <c r="E113" s="13">
+        <f t="shared" si="3"/>
+        <v>35.62988</v>
+      </c>
+      <c r="F113" s="11">
+        <v>29.8</v>
+      </c>
+      <c r="G113">
+        <v>24</v>
+      </c>
+      <c r="I113" s="13">
+        <f t="shared" si="4"/>
+        <v>20.33154</v>
+      </c>
+      <c r="J113" s="13">
+        <f t="shared" si="5"/>
+        <v>-9.4684600000000003</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>66</v>
+      </c>
+      <c r="B114" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D114" s="11">
+        <v>1.5045999999999999</v>
+      </c>
+      <c r="E114" s="13">
+        <f t="shared" si="3"/>
+        <v>34.708280000000002</v>
+      </c>
+      <c r="F114" s="11">
+        <v>28.8</v>
+      </c>
+      <c r="G114">
+        <v>24</v>
+      </c>
+      <c r="I114" s="13">
+        <f t="shared" si="4"/>
+        <v>19.358740000000001</v>
+      </c>
+      <c r="J114" s="13">
+        <f t="shared" si="5"/>
+        <v>-9.4412599999999998</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="B3:C5">
-    <sortCondition ref="B2"/>
+  <sortState ref="A69:J106">
+    <sortCondition ref="A68"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>